<commit_message>
Changed path to data
</commit_message>
<xml_diff>
--- a/Data/any_data/count.xlsx
+++ b/Data/any_data/count.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsavvin\Desktop\programm2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsavvin\Desktop\programm2\Data\any_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -397,10 +397,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,50 +428,72 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="C2" s="3">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
-        <v>0.29166666666666669</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="B3" s="6">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="C3" s="3">
-        <v>80</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
+        <v>0.375</v>
+      </c>
+      <c r="B4" s="6">
         <v>0.5</v>
       </c>
-      <c r="B4" s="6">
-        <v>0.75</v>
-      </c>
       <c r="C4" s="3">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="B5" s="6">
-        <v>0.875</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C5" s="3">
-        <v>200</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
-        <v>0.875</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="B6" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="C6" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
+        <v>0.75</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C7" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="B8" s="4">
         <v>0</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C8" s="5">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added legend and  title to graphs
</commit_message>
<xml_diff>
--- a/Data/any_data/count.xlsx
+++ b/Data/any_data/count.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18190" windowHeight="8510"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -400,16 +400,16 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -420,18 +420,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>0</v>
       </c>
       <c r="B2" s="6">
-        <v>0.29166666666666669</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="C2" s="3">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>0.27083333333333331</v>
       </c>
@@ -442,7 +442,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>0.375</v>
       </c>
@@ -453,7 +453,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>0.5</v>
       </c>
@@ -464,7 +464,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>0.66666666666666663</v>
       </c>
@@ -475,7 +475,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>0.75</v>
       </c>
@@ -486,7 +486,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>0.91666666666666663</v>
       </c>

</xml_diff>